<commit_message>
Trying to read data from excel - unsuccessful
</commit_message>
<xml_diff>
--- a/DesignPattern/DataDrivenTests/UserData.xlsx
+++ b/DesignPattern/DataDrivenTests/UserData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -14,54 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>martialStatus</t>
-  </si>
-  <si>
-    <t>hobbies</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>birthMonth</t>
-  </si>
-  <si>
-    <t>birthDay</t>
-  </si>
-  <si>
-    <t>birthYear</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>picture</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>confirmPassword</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Iliya</t>
+  </si>
+  <si>
+    <t>RegisterWithoutLastName</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Iliev</t>
   </si>
 </sst>
 </file>
@@ -77,18 +47,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -103,9 +67,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,35 +373,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -446,52 +396,20 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E2" s="1">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Trying to fix oledb connection [unsuccessful]
</commit_message>
<xml_diff>
--- a/DesignPattern/DataDrivenTests/UserData.xlsx
+++ b/DesignPattern/DataDrivenTests/UserData.xlsx
@@ -14,13 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Iliya</t>
-  </si>
-  <si>
-    <t>RegisterWithoutLastName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Key</t>
   </si>
@@ -28,10 +22,10 @@
     <t>FirstName</t>
   </si>
   <si>
-    <t>LastName</t>
+    <t>RegisterWithoutLastName</t>
   </si>
   <si>
-    <t>Iliev</t>
+    <t>Iliya</t>
   </si>
 </sst>
 </file>
@@ -373,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,26 +380,20 @@
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Connection with excel file is established but cannot take data
</commit_message>
<xml_diff>
--- a/DesignPattern/DataDrivenTests/UserData.xlsx
+++ b/DesignPattern/DataDrivenTests/UserData.xlsx
@@ -14,18 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>RegisterWithoutLastName</t>
   </si>
   <si>
-    <t>Iliya</t>
+    <t>key</t>
+  </si>
+  <si>
+    <t>this.firstName</t>
   </si>
 </sst>
 </file>
@@ -370,7 +367,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,18 +379,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create property "Key" for user
</commit_message>
<xml_diff>
--- a/DesignPattern/DataDrivenTests/UserData.xlsx
+++ b/DesignPattern/DataDrivenTests/UserData.xlsx
@@ -14,15 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
   <si>
     <t>RegisterWithoutLastName</t>
   </si>
   <si>
-    <t>key</t>
+    <t>Iliya</t>
   </si>
   <si>
-    <t>this.firstName</t>
+    <t>LastName</t>
   </si>
 </sst>
 </file>
@@ -364,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,17 +383,23 @@
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fill whole excel file
</commit_message>
<xml_diff>
--- a/DesignPattern/DataDrivenTests/UserData.xlsx
+++ b/DesignPattern/DataDrivenTests/UserData.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Key</t>
   </si>
@@ -29,16 +29,96 @@
   </si>
   <si>
     <t>LastName</t>
+  </si>
+  <si>
+    <t>MartialStatus</t>
+  </si>
+  <si>
+    <t>Hobbies</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>BirthMonth</t>
+  </si>
+  <si>
+    <t>BirthDay</t>
+  </si>
+  <si>
+    <t>BirthYear</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Picture</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>0897675645</t>
+  </si>
+  <si>
+    <t>lichkata456</t>
+  </si>
+  <si>
+    <t>lichkata456@abv.bg</t>
+  </si>
+  <si>
+    <t>C:\Users\Iliya\Desktop\photo.jpeg</t>
+  </si>
+  <si>
+    <t>ALA BALA</t>
+  </si>
+  <si>
+    <t>12345678</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -61,13 +141,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -370,40 +454,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update all only to test with first and last name
</commit_message>
<xml_diff>
--- a/DesignPattern/DataDrivenTests/UserData.xlsx
+++ b/DesignPattern/DataDrivenTests/UserData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Key</t>
   </si>
@@ -29,78 +29,6 @@
   </si>
   <si>
     <t>LastName</t>
-  </si>
-  <si>
-    <t>MartialStatus</t>
-  </si>
-  <si>
-    <t>Hobbies</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>BirthMonth</t>
-  </si>
-  <si>
-    <t>BirthDay</t>
-  </si>
-  <si>
-    <t>BirthYear</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Picture</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>ConfirmPassword</t>
-  </si>
-  <si>
-    <t>1,2,3</t>
-  </si>
-  <si>
-    <t>Bulgaria</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>1987</t>
-  </si>
-  <si>
-    <t>0897675645</t>
-  </si>
-  <si>
-    <t>lichkata456</t>
-  </si>
-  <si>
-    <t>lichkata456@abv.bg</t>
-  </si>
-  <si>
-    <t>C:\Users\Iliya\Desktop\photo.jpeg</t>
-  </si>
-  <si>
-    <t>ALA BALA</t>
-  </si>
-  <si>
-    <t>12345678</t>
   </si>
   <si>
     <t>String.Empty</t>
@@ -110,18 +38,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,18 +64,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,18 +386,10 @@
     <col min="1" max="1" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,101 +399,20 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>28</v>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Filling the form with everything except the lists
</commit_message>
<xml_diff>
--- a/DesignPattern/DataDrivenTests/UserData.xlsx
+++ b/DesignPattern/DataDrivenTests/UserData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Key</t>
   </si>
@@ -32,16 +32,87 @@
   </si>
   <si>
     <t>String.Empty</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>BirthMonth</t>
+  </si>
+  <si>
+    <t>BirthDay</t>
+  </si>
+  <si>
+    <t>BirthYear</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Picture</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>0897675645</t>
+  </si>
+  <si>
+    <t>lichkata456</t>
+  </si>
+  <si>
+    <t>lichkata456@abv.bg</t>
+  </si>
+  <si>
+    <t>C:\Users\Iliya\Desktop\photo.jpeg</t>
+  </si>
+  <si>
+    <t>ALA BALA</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -64,15 +135,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -375,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,10 +459,18 @@
     <col min="1" max="1" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -399,20 +480,89 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implementing check for typing String.Empty
</commit_message>
<xml_diff>
--- a/DesignPattern/DataDrivenTests/UserData.xlsx
+++ b/DesignPattern/DataDrivenTests/UserData.xlsx
@@ -31,70 +31,70 @@
     <t>LastName</t>
   </si>
   <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>BirthMonth</t>
+  </si>
+  <si>
+    <t>BirthDay</t>
+  </si>
+  <si>
+    <t>BirthYear</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Picture</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1987</t>
+  </si>
+  <si>
+    <t>0897675645</t>
+  </si>
+  <si>
+    <t>lichkata456</t>
+  </si>
+  <si>
+    <t>lichkata456@abv.bg</t>
+  </si>
+  <si>
+    <t>C:\Users\Iliya\Desktop\photo.jpeg</t>
+  </si>
+  <si>
+    <t>ALA BALA</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
     <t>String.Empty</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>BirthMonth</t>
-  </si>
-  <si>
-    <t>BirthDay</t>
-  </si>
-  <si>
-    <t>BirthYear</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Picture</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>ConfirmPassword</t>
-  </si>
-  <si>
-    <t>Bulgaria</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>1987</t>
-  </si>
-  <si>
-    <t>0897675645</t>
-  </si>
-  <si>
-    <t>lichkata456</t>
-  </si>
-  <si>
-    <t>lichkata456@abv.bg</t>
-  </si>
-  <si>
-    <t>C:\Users\Iliya\Desktop\photo.jpeg</t>
-  </si>
-  <si>
-    <t>ALA BALA</t>
-  </si>
-  <si>
-    <t>12345678</t>
-  </si>
-  <si>
-    <t>23</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,37 +481,37 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -522,40 +522,40 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementing logic for clicking on checkboxes and radio buttons
</commit_message>
<xml_diff>
--- a/DesignPattern/DataDrivenTests/UserData.xlsx
+++ b/DesignPattern/DataDrivenTests/UserData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Key</t>
   </si>
@@ -94,7 +94,19 @@
     <t>23</t>
   </si>
   <si>
-    <t>String.Empty</t>
+    <t>Iliev</t>
+  </si>
+  <si>
+    <t>MartialStatus</t>
+  </si>
+  <si>
+    <t>Hobbies</t>
+  </si>
+  <si>
+    <t>false false true</t>
+  </si>
+  <si>
+    <t>false false false</t>
   </si>
 </sst>
 </file>
@@ -448,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,18 +471,19 @@
     <col min="1" max="1" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="5" width="13.85546875" style="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,40 +494,46 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -525,42 +544,48 @@
         <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
First negative test with Data Driven Test approach
</commit_message>
<xml_diff>
--- a/DesignPattern/DataDrivenTests/UserData.xlsx
+++ b/DesignPattern/DataDrivenTests/UserData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Key</t>
   </si>
@@ -94,19 +94,16 @@
     <t>23</t>
   </si>
   <si>
-    <t>Iliev</t>
-  </si>
-  <si>
     <t>MartialStatus</t>
   </si>
   <si>
     <t>Hobbies</t>
   </si>
   <si>
-    <t>false false true</t>
-  </si>
-  <si>
-    <t>false false false</t>
+    <t>String.Empty</t>
+  </si>
+  <si>
+    <t>true true true</t>
   </si>
 </sst>
 </file>
@@ -463,7 +460,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,10 +491,10 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -541,10 +538,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Add ten negative tests against the registration form
</commit_message>
<xml_diff>
--- a/DesignPattern/DataDrivenTests/UserData.xlsx
+++ b/DesignPattern/DataDrivenTests/UserData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="540"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="48">
   <si>
     <t>Key</t>
   </si>
@@ -104,6 +104,60 @@
   </si>
   <si>
     <t>true true true</t>
+  </si>
+  <si>
+    <t>RegisterWithoutHobby</t>
+  </si>
+  <si>
+    <t>lichkata457</t>
+  </si>
+  <si>
+    <t>Iliev</t>
+  </si>
+  <si>
+    <t>false false false</t>
+  </si>
+  <si>
+    <t>RegisterWithoutPhone</t>
+  </si>
+  <si>
+    <t>false false true</t>
+  </si>
+  <si>
+    <t>RegisterWithShortPhone</t>
+  </si>
+  <si>
+    <t>088</t>
+  </si>
+  <si>
+    <t>RegisterWithLongPhone</t>
+  </si>
+  <si>
+    <t>08823445671787895656556566556</t>
+  </si>
+  <si>
+    <t>RegisterWithoutUsername</t>
+  </si>
+  <si>
+    <t>RegisterWithoutEmail</t>
+  </si>
+  <si>
+    <t>RegisterWithWrongEmail</t>
+  </si>
+  <si>
+    <t>lichkata456@abv.</t>
+  </si>
+  <si>
+    <t>RegisterWithoutPassword</t>
+  </si>
+  <si>
+    <t>RegisterWithoutConfirmationPassword</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>RegisterWithShortPassword</t>
   </si>
 </sst>
 </file>
@@ -148,10 +202,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -457,25 +512,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.85546875" style="1" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -580,11 +638,520 @@
         <v>24</v>
       </c>
     </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L3" r:id="rId2"/>
+    <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="L5" r:id="rId4"/>
+    <hyperlink ref="L6" r:id="rId5"/>
+    <hyperlink ref="L7" r:id="rId6"/>
+    <hyperlink ref="L9" r:id="rId7"/>
+    <hyperlink ref="L10" r:id="rId8"/>
+    <hyperlink ref="L11" r:id="rId9"/>
+    <hyperlink ref="L12" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more negative tests added
</commit_message>
<xml_diff>
--- a/DesignPattern/DataDrivenTests/UserData.xlsx
+++ b/DesignPattern/DataDrivenTests/UserData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="65">
   <si>
     <t>Key</t>
   </si>
@@ -154,10 +154,61 @@
     <t>RegisterWithoutConfirmationPassword</t>
   </si>
   <si>
+    <t>12345679</t>
+  </si>
+  <si>
     <t>1234567</t>
   </si>
   <si>
     <t>RegisterWithShortPassword</t>
+  </si>
+  <si>
+    <t>RegisterWithUnmatchedPasswords</t>
+  </si>
+  <si>
+    <t>RegisterWithoutLastNameAndPhone</t>
+  </si>
+  <si>
+    <t>RegisterWithoutLastNameAndUsername</t>
+  </si>
+  <si>
+    <t>RegisterWithoutLastNameAndEmail</t>
+  </si>
+  <si>
+    <t>RegisterWithoutLastNameAndWrongEmail</t>
+  </si>
+  <si>
+    <t>RegisterWithoutHobbiesAndUsername</t>
+  </si>
+  <si>
+    <t>RegisterWithoutUsernameAndPassword</t>
+  </si>
+  <si>
+    <t>false true false</t>
+  </si>
+  <si>
+    <t>RegisterWithNegativePhone</t>
+  </si>
+  <si>
+    <t>0897675646</t>
+  </si>
+  <si>
+    <t>-0897675646</t>
+  </si>
+  <si>
+    <t>RegisterWithNegativePhoneAndWrongEmail</t>
+  </si>
+  <si>
+    <t>RegisterWithWrongEmailAndMismatchedPasswords</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>RegisterWithWrongEmailAndMismatchedAndShortPasswords</t>
+  </si>
+  <si>
+    <t>RegisterAlreadyRegisteredUser</t>
   </si>
 </sst>
 </file>
@@ -512,15 +563,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" style="1" customWidth="1"/>
@@ -1090,7 +1141,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -1132,9 +1183,609 @@
         <v>23</v>
       </c>
       <c r="O12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P12" s="1" t="s">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P24" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1150,8 +1801,19 @@
     <hyperlink ref="L10" r:id="rId8"/>
     <hyperlink ref="L11" r:id="rId9"/>
     <hyperlink ref="L12" r:id="rId10"/>
+    <hyperlink ref="L13" r:id="rId11"/>
+    <hyperlink ref="L14" r:id="rId12"/>
+    <hyperlink ref="L15" r:id="rId13"/>
+    <hyperlink ref="L17" r:id="rId14"/>
+    <hyperlink ref="L18" r:id="rId15"/>
+    <hyperlink ref="L19" r:id="rId16"/>
+    <hyperlink ref="L20" r:id="rId17"/>
+    <hyperlink ref="L21" r:id="rId18"/>
+    <hyperlink ref="L22" r:id="rId19"/>
+    <hyperlink ref="L23" r:id="rId20"/>
+    <hyperlink ref="L24" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>